<commit_message>
finished some of reporting
</commit_message>
<xml_diff>
--- a/src/routers/projects.xlsx
+++ b/src/routers/projects.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>project ID</t>
   </si>
@@ -65,6 +65,60 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Actual Spend Total</t>
+  </si>
+  <si>
+    <t>fixedPrice/2023-08-24T08:30:26.178Z/client2</t>
+  </si>
+  <si>
+    <t>newProject</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>fixedPrice</t>
+  </si>
+  <si>
+    <t>notStarted</t>
+  </si>
+  <si>
+    <t>Ahmed shalaab</t>
+  </si>
+  <si>
+    <t>client2pm</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>referenceNumber1</t>
+  </si>
+  <si>
+    <t>client2</t>
+  </si>
+  <si>
+    <t>TnM/3122-06-12T11:31:00Z/client1</t>
+  </si>
+  <si>
+    <t>iprojectnase</t>
+  </si>
+  <si>
+    <t>TnM</t>
+  </si>
+  <si>
+    <t>obaid saafan</t>
+  </si>
+  <si>
+    <t>client1pm</t>
+  </si>
+  <si>
+    <t>client1</t>
   </si>
 </sst>
 </file>
@@ -100,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,6 +553,106 @@
       </c>
       <c r="R1" t="s">
         <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45162.35446965278</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2">
+        <v>35234</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2">
+        <v>12345</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1">
+        <v>446490.4798611111</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3">
+        <v>35234</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3">
+        <v>12345</v>
+      </c>
+      <c r="P3">
+        <v>12345</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3">
+        <v>56000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experimented with project reports in test router
</commit_message>
<xml_diff>
--- a/src/routers/projects.xlsx
+++ b/src/routers/projects.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Projects" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Profile" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t>project ID</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Project Status</t>
   </si>
   <si>
-    <t>Project Start Date</t>
+    <t xml:space="preserve">Project Start Date </t>
   </si>
   <si>
     <t>Project Manager</t>
@@ -67,10 +67,130 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Actual Spend Total</t>
-  </si>
-  <si>
-    <t>Revenue recognized</t>
+    <t>Actual Spend</t>
+  </si>
+  <si>
+    <t>Total Revenue recognized</t>
+  </si>
+  <si>
+    <t>fixedPrice/2023-08-24T08:30:35.773Z/client2</t>
+  </si>
+  <si>
+    <t>project element</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>fixedPrice</t>
+  </si>
+  <si>
+    <t>inProgress</t>
+  </si>
+  <si>
+    <t>2023-08-24T08:30:35.773Z</t>
+  </si>
+  <si>
+    <t>Ahmed Shalaab</t>
+  </si>
+  <si>
+    <t>client2pm</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>referenceNumber1</t>
+  </si>
+  <si>
+    <t>client2</t>
+  </si>
+  <si>
+    <t>TnM/2023-08-24T10:33:33.752Z/client1</t>
+  </si>
+  <si>
+    <t>iprojectnase2</t>
+  </si>
+  <si>
+    <t>TnM</t>
+  </si>
+  <si>
+    <t>onHold</t>
+  </si>
+  <si>
+    <t>2023-08-24T10:33:33.752Z</t>
+  </si>
+  <si>
+    <t>obaid saafan</t>
+  </si>
+  <si>
+    <t>client1pm</t>
+  </si>
+  <si>
+    <t>referenceNumber2</t>
+  </si>
+  <si>
+    <t>client1</t>
+  </si>
+  <si>
+    <t>TnM/2023-09-16T17:30:36.885Z/client1</t>
+  </si>
+  <si>
+    <t>iprojectndse2</t>
+  </si>
+  <si>
+    <t>notStarted</t>
+  </si>
+  <si>
+    <t>2023-09-16T17:30:36.885Z</t>
+  </si>
+  <si>
+    <t>fixedPrice/2023-08-24T08:30:01.277Z/client2</t>
+  </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>2023-08-24T08:30:01.277Z</t>
+  </si>
+  <si>
+    <t>fixedPrice/2023-08-28T08:15:58.241Z/client2</t>
+  </si>
+  <si>
+    <t>project element new</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>2023-08-28T08:15:58.241Z</t>
+  </si>
+  <si>
+    <t>fixedPrice/2023-08-24T08:30:26.178Z/client2</t>
+  </si>
+  <si>
+    <t>newProject</t>
+  </si>
+  <si>
+    <t>2023-08-24T08:30:26.178Z</t>
+  </si>
+  <si>
+    <t>TnM/3122-06-12T11:31:00Z/client1</t>
+  </si>
+  <si>
+    <t>iprojectnase</t>
+  </si>
+  <si>
+    <t>3122-06-12T11:31:00.000Z</t>
+  </si>
+  <si>
+    <t>AED</t>
   </si>
 </sst>
 </file>
@@ -447,8 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="20" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -510,6 +633,317 @@
       </c>
       <c r="T1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2">
+        <v>35234</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>12345</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3">
+        <v>35234</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3">
+        <v>12345</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>35234</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4">
+        <v>12345</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>35234</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>12345</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>35234</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6">
+        <v>12345</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7">
+        <v>35234</v>
+      </c>
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7">
+        <v>12345</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8">
+        <v>35234</v>
+      </c>
+      <c r="M8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8">
+        <v>12345</v>
+      </c>
+      <c r="P8">
+        <v>12345</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>